<commit_message>
reading in rest of file works
</commit_message>
<xml_diff>
--- a/DataOut.xlsx
+++ b/DataOut.xlsx
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
finished set up editted sheet
</commit_message>
<xml_diff>
--- a/DataOut.xlsx
+++ b/DataOut.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>Co-OpID</t>
   </si>
@@ -182,6 +182,63 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>MUID</t>
+  </si>
+  <si>
+    <t>TERM</t>
+  </si>
+  <si>
+    <t>COMPANY_ID</t>
+  </si>
+  <si>
+    <t>ACTIVITY</t>
+  </si>
+  <si>
+    <t>SALARY</t>
+  </si>
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>COUNTRY</t>
+  </si>
+  <si>
+    <t>REGID</t>
+  </si>
+  <si>
+    <t>WORK_REG</t>
+  </si>
+  <si>
+    <t>WORK_GRADE</t>
+  </si>
+  <si>
+    <t>GRADING_REG</t>
+  </si>
+  <si>
+    <t>GRADING_GRADE</t>
+  </si>
+  <si>
+    <t>EMPLOYER_EVAL_DATE</t>
+  </si>
+  <si>
+    <t>EMPLOYER_EVAL</t>
+  </si>
+  <si>
+    <t>EMPLOYER_AUTH</t>
+  </si>
+  <si>
+    <t>STUDENT_EVAL_DATE</t>
+  </si>
+  <si>
+    <t>STUDENT_EVAL</t>
   </si>
 </sst>
 </file>
@@ -1584,12 +1641,75 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>70</v>
+      </c>
+      <c r="R1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S1" t="s">
+        <v>72</v>
+      </c>
+      <c r="T1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
took out 2d array, before clean up
</commit_message>
<xml_diff>
--- a/DataOut.xlsx
+++ b/DataOut.xlsx
@@ -1,15 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19125"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kathleenbaert/Documents/workspace/IRDatabase/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr documentId="8_{55B21C2C-7271-4923-8FBE-7FA792675F93}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="30" xr6:coauthVersionMax="30"/>
   <bookViews>
-    <workbookView windowHeight="8020" windowWidth="14800" xWindow="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="460"/>
+    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -244,11 +240,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -596,16 +592,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="AV2" sqref="AV2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -748,7 +742,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:47">
       <c r="A2">
         <v>1365</v>
       </c>
@@ -804,7 +798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:47">
       <c r="A3">
         <v>1366</v>
       </c>
@@ -857,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:47">
       <c r="A4">
         <v>1368</v>
       </c>
@@ -913,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:47">
       <c r="A5">
         <v>1362</v>
       </c>
@@ -933,7 +927,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:47">
       <c r="A6">
         <v>1363</v>
       </c>
@@ -953,7 +947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:47">
       <c r="A7">
         <v>1364</v>
       </c>
@@ -997,7 +991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:47">
       <c r="A8">
         <v>1367</v>
       </c>
@@ -1038,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:47">
       <c r="A9">
         <v>1367</v>
       </c>
@@ -1079,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:47">
       <c r="A10">
         <v>1367</v>
       </c>
@@ -1120,7 +1114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:47">
       <c r="A11">
         <v>1369</v>
       </c>
@@ -1161,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:47">
       <c r="A12">
         <v>1370</v>
       </c>
@@ -1181,7 +1175,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:47">
       <c r="A13">
         <v>3826</v>
       </c>
@@ -1237,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:47">
       <c r="A14">
         <v>3827</v>
       </c>
@@ -1293,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:47">
       <c r="A15">
         <v>3827</v>
       </c>
@@ -1349,7 +1343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:47">
       <c r="A16">
         <v>3830</v>
       </c>
@@ -1429,7 +1423,7 @@
         <v>43151</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:47">
       <c r="A17">
         <v>3830</v>
       </c>
@@ -1509,7 +1503,7 @@
         <v>43151</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:47">
       <c r="A18">
         <v>3828</v>
       </c>
@@ -1550,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:47">
       <c r="A19">
         <v>3829</v>
       </c>
@@ -1570,7 +1564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:47">
       <c r="A20">
         <v>3831</v>
       </c>
@@ -1614,7 +1608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:47">
       <c r="A21">
         <v>3832</v>
       </c>

</xml_diff>

<commit_message>
added transferring coop info
</commit_message>
<xml_diff>
--- a/DataOut.xlsx
+++ b/DataOut.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
   <si>
     <t>Co-OpID</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>STUDENT_EVAL</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -764,6 +767,9 @@
       <c r="G2" s="1">
         <v>21</v>
       </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
       <c r="L2">
         <v>39442</v>
       </c>
@@ -817,6 +823,10 @@
       <c r="F3">
         <v>1</v>
       </c>
+      <c r="G3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
       <c r="L3">
         <v>39443</v>
       </c>
@@ -873,6 +883,9 @@
       <c r="G4" s="1">
         <v>23</v>
       </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
       <c r="L4">
         <v>39445</v>
       </c>
@@ -971,6 +984,9 @@
       <c r="G7" s="1">
         <v>21</v>
       </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
       <c r="L7">
         <v>39441</v>
       </c>
@@ -1199,6 +1215,9 @@
       <c r="G13" s="1">
         <v>15</v>
       </c>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
       <c r="L13">
         <v>40587</v>
       </c>
@@ -1255,6 +1274,9 @@
       <c r="G14" s="1">
         <v>15</v>
       </c>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
       <c r="L14">
         <v>46900</v>
       </c>
@@ -1311,6 +1333,9 @@
       <c r="G15" s="1">
         <v>15</v>
       </c>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
       <c r="L15">
         <v>47172</v>
       </c>
@@ -1367,6 +1392,9 @@
       <c r="G16" s="1">
         <v>16</v>
       </c>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
       <c r="L16">
         <v>40590</v>
       </c>
@@ -1447,6 +1475,9 @@
       <c r="G17" s="1">
         <v>16</v>
       </c>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
       <c r="L17">
         <v>40590</v>
       </c>
@@ -1638,7 +1669,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1706,6 +1737,321 @@
         <v>71</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1365.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>5509033.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1621.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" t="n">
+        <v>39442.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>3993.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1366.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5509033.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1621.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" t="n">
+        <v>39443.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>4991.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1368.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5509033.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1621.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" t="n">
+        <v>39445.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4993.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1364.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>5509033.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1621.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" t="n">
+        <v>39441.0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>3991.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3826.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5735207.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1562.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" t="n">
+        <v>40587.0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>3991.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3827.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>5735207.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1562.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" t="n">
+        <v>46900.0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>3992.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3827.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>5735207.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1562.0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" t="n">
+        <v>47172.0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>3993.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>3830.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>5735207.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1562.0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" t="n">
+        <v>40590.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>4991.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>3830.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>5735207.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1562.0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" t="n">
+        <v>40590.0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>4991.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>